<commit_message>
Update connectsome of C elegans.xlsx
</commit_message>
<xml_diff>
--- a/connectsome of C elegans/result/connectsome of C elegans.xlsx
+++ b/connectsome of C elegans/result/connectsome of C elegans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1_learning\2_class\9_2022_Fall\computational neuroscience\homework_by_me\homework_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Public_repository\coding-homework-of-C-Neuro\connectsome of C elegans\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52121137-6EAA-4BAD-A3FD-C221A902543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB33F1E-BD0D-4A52-B73E-F0538E54CA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="motif_2" sheetId="2" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -150,6 +147,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -434,90 +434,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9270B4-34D9-45A3-92A8-EE60425D8A42}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="5"/>
-    <col min="2" max="2" width="33.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="7"/>
-    <col min="6" max="6" width="8.6640625" style="5"/>
-    <col min="7" max="16384" width="8.6640625" style="6"/>
+    <col min="1" max="1" width="8.6640625" style="4"/>
+    <col min="2" max="2" width="33.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="6"/>
+    <col min="6" max="6" width="8.6640625" style="4"/>
+    <col min="7" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>187</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>55.5</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>6.5</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <f>(B2-C2)/D2</f>
         <v>20.23076923076923</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f>B2/C2</f>
         <v>3.3693693693693691</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1731</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1994.1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>13.1</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <f>(B3-C3)/D3</f>
         <v>-20.083969465648849</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f>B3/C3</f>
         <v>0.86806077929893188</v>
       </c>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -548,7 +548,7 @@
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="2"/>
     <col min="6" max="6" width="8.6640625" style="1"/>
-    <col min="7" max="7" width="8.6640625" style="8"/>
+    <col min="7" max="7" width="8.6640625" style="7"/>
     <col min="8" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -571,131 +571,131 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>238</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>16</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>2.6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>1.6</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="8">
         <f t="shared" ref="E2:E14" si="0">(B2-C2)/D2</f>
         <v>8.375</v>
       </c>
       <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f t="shared" ref="G2:G14" si="1">B2/C2</f>
         <v>6.1538461538461533</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>108</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>487</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>128</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>11</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <f t="shared" si="0"/>
         <v>32.636363636363633</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f t="shared" si="1"/>
         <v>3.8046875</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>46</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>299</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>85</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>9</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <f t="shared" si="0"/>
         <v>23.777777777777779</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f t="shared" si="1"/>
         <v>3.5176470588235293</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>110</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>139</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>48</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>6</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
         <v>15.166666666666666</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <f t="shared" si="1"/>
         <v>2.8958333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>38</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>1521</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>894</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>34</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>18.441176470588236</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <f t="shared" si="1"/>
         <v>1.7013422818791946</v>
       </c>
@@ -717,10 +717,10 @@
         <f t="shared" si="0"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <f t="shared" si="1"/>
         <v>1.1724137931034482</v>
       </c>
@@ -745,7 +745,7 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f t="shared" si="1"/>
         <v>0.96569688226336459</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <f t="shared" si="1"/>
         <v>0.89749847467968269</v>
       </c>
@@ -795,7 +795,7 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f t="shared" si="1"/>
         <v>0.89137873937520695</v>
       </c>
@@ -820,7 +820,7 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <f t="shared" si="1"/>
         <v>0.81454918032786883</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f t="shared" si="1"/>
         <v>0.75988455988455983</v>
       </c>
@@ -870,7 +870,7 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <f t="shared" si="1"/>
         <v>0.68203883495145634</v>
       </c>
@@ -895,7 +895,7 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <f t="shared" si="1"/>
         <v>0.47517730496453903</v>
       </c>

</xml_diff>